<commit_message>
Added increased support for the creation and reporting of imputed values
</commit_message>
<xml_diff>
--- a/examples/Olink_Finished_Example/data/raw/Fake_Example_Olink_Data.xlsx
+++ b/examples/Olink_Finished_Example/data/raw/Fake_Example_Olink_Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pelowitz.thomas/Documents/Analysis_Pipeline_Textual/examples/Olink_Finished_Example/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FED54EB-2187-3444-A959-861E8C81E01A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0350DB5-1ACF-4D43-AA86-C7F92F97D3A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1240" windowWidth="34560" windowHeight="19600" xr2:uid="{7909AE00-1EC4-6B48-A589-D037E95155A9}"/>
   </bookViews>
@@ -1245,7 +1245,7 @@
   <dimension ref="A1:L45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1495,9 +1495,7 @@
       <c r="F7" s="15">
         <v>0.44336009050000058</v>
       </c>
-      <c r="G7" s="16">
-        <v>0.14648556750000011</v>
-      </c>
+      <c r="G7" s="16"/>
       <c r="H7" s="15">
         <v>0.76951384550000057</v>
       </c>
@@ -1732,9 +1730,7 @@
       <c r="I13" s="16">
         <v>0.52506685300000022</v>
       </c>
-      <c r="J13" s="15">
-        <v>0.14729928999999939</v>
-      </c>
+      <c r="J13" s="15"/>
       <c r="K13" s="16">
         <v>-0.15536212900000021</v>
       </c>

</xml_diff>